<commit_message>
added excel sheet for log
</commit_message>
<xml_diff>
--- a/data/humidity_log.xlsx
+++ b/data/humidity_log.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\Documents\Projects\NWA_Sensors\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFC4964-C82A-4228-9DE5-8F4D0568EA29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4016087-892E-40AE-825A-E41F10C5D143}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{299EE807-B36D-48F9-9004-BE24E6545448}"/>
   </bookViews>
@@ -46,8 +46,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -78,19 +79,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+      <numFmt numFmtId="168" formatCode="dd/mm/yyyy\ hh:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ am/pm"/>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
@@ -439,112 +441,112 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="1" t="str">
-        <f t="shared" ref="B2:B17" ca="1" si="0">IF(A2&lt;&gt;"",IF(B2&lt;&gt;"",B2,NOW()),"")</f>
+      <c r="B2" s="2" t="str">
+        <f ca="1">IF(A2&lt;&gt;"",IF(B2&lt;&gt;"",B2,NOW()),"")</f>
         <v/>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="1" t="str">
-        <f t="shared" ca="1" si="0"/>
+      <c r="B3" s="2" t="str">
+        <f t="shared" ref="B2:B17" ca="1" si="0">IF(A3&lt;&gt;"",IF(B3&lt;&gt;"",B3,NOW()),"")</f>
         <v/>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="1" t="str">
+      <c r="B4" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="1" t="str">
+      <c r="B5" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="1" t="str">
+      <c r="B6" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="1" t="str">
+      <c r="B7" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="1" t="str">
+      <c r="B8" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="1" t="str">
+      <c r="B9" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="1" t="str">
+      <c r="B10" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="1" t="str">
+      <c r="B11" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="str">
+      <c r="B12" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="1" t="str">
+      <c r="B13" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="1" t="str">
+      <c r="B14" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="1" t="str">
+      <c r="B15" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="1" t="str">
+      <c r="B16" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="1" t="str">
+      <c r="B17" s="2" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>

</xml_diff>